<commit_message>
make workflow, enhance code quality
</commit_message>
<xml_diff>
--- a/OCR/pilot_data_ocr1.xlsx
+++ b/OCR/pilot_data_ocr1.xlsx
@@ -441,12 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>filename</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>ocr</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>filename</t>
         </is>
       </c>
     </row>

</xml_diff>